<commit_message>
ADD CRUD in the first Window
</commit_message>
<xml_diff>
--- a/basedatosPrueba.xlsx
+++ b/basedatosPrueba.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
@@ -537,6 +537,33 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Jesus</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Alexander Benitez</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1458789</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1728224557</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Dr. Atiencia Atiencia Atiencia Atiencia</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ADD completed the two tables and finished the CRUD V1.3
I completed the logic for the two tables, with a simple CRUD that someone can put information in the first table and with a double click in the dates you can visualize a second windows with more dates and a complete table.
</commit_message>
<xml_diff>
--- a/basedatosPrueba.xlsx
+++ b/basedatosPrueba.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
@@ -540,7 +540,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Jesus</t>
+          <t>Alberto Gomez</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -561,6 +561,60 @@
       <c r="E4" t="inlineStr">
         <is>
           <t>Dr. Atiencia Atiencia Atiencia Atiencia</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Phd. Christian Suarez</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Raul Alejandro Sosa</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>172845688978</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1548785225</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Dr. Christian Santiago Izurieta Cruz</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Lic. Pedro Peralta</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Josue Alberto Ramirez Arboleda</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>174578569933</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1245785689</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Dr. Christian Santiago Izurieta Cruz</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
ADD all the principal elements that I program
</commit_message>
<xml_diff>
--- a/basedatosPrueba.xlsx
+++ b/basedatosPrueba.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
@@ -636,7 +636,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1728220441</t>
+          <t>1245789663</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -648,22 +648,22 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Ing. AAAA</t>
+          <t>Lic. Albertino Jesus Heredia Paez</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>AAAA</t>
+          <t>Alexander Francisco Tibanta Miranda</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>123456789</t>
+          <t>1728220441001</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>456789123</t>
+          <t>1728220441</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -675,52 +675,25 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Lic. Albertino Jesus Heredia Paez</t>
+          <t>Lic. Alexander Javier Miranda Granero</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Alexander Francisco Tibanta Miranda</t>
+          <t>Peter Patricio Tene Ojeda</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1728220441001</t>
+          <t>174582556</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1728220441</t>
+          <t>174582556001</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
-        <is>
-          <t>Dr. Christian Santiago Izurieta Cruz</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Lic. Alexander Javier Miranda Granero</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Peter Patricio Tene Ojeda</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>174582556</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>174582556001</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
         <is>
           <t>Dr. Christian Santiago Izurieta Cruz</t>
         </is>

</xml_diff>